<commit_message>
Fix the one-var data tables.
The column and row input cell references were flipped.
</commit_message>
<xml_diff>
--- a/test/xlsx/data-table/one-variable.xlsx
+++ b/test/xlsx/data-table/one-variable.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -462,15 +462,15 @@
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <f t="dataTable" ref="B5:B11" dt2D="0" dtr="1" r1="A2" ca="1"/>
-        <v>1</v>
+        <f t="dataTable" ref="B5:B11" dt2D="0" dtr="0" r1="A2"/>
+        <v>2</v>
       </c>
       <c r="D5" s="3">
         <f>C2</f>
         <v>2</v>
       </c>
       <c r="E5" s="4">
-        <f t="dataTable" ref="E5:I5" dt2D="0" dtr="0" r1="B2" ca="1"/>
+        <f t="dataTable" ref="E5:I5" dt2D="0" dtr="1" r1="B2" ca="1"/>
         <v>10</v>
       </c>
       <c r="F5" s="4">
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -515,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -523,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -531,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="4">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>